<commit_message>
Update polynomial regression; include instance ID in the hierarchical index; remove the features 'Distance To Closest Other Cluster Ratio' and 'Cluster' from the TSP dataset; compute final results
</commit_message>
<xml_diff>
--- a/03_tuning_results/c_CVRP_tuning_details.xlsx
+++ b/03_tuning_results/c_CVRP_tuning_details.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,20 +441,25 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>PR</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>RF</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>XGBoost</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>KM</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>NN</t>
         </is>
@@ -473,20 +478,25 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>GridSearchCV</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>RandomizedSearchCV</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>GridSearchCV</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>GridSearchCV</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>GridSearchCV</t>
         </is>
@@ -502,15 +512,18 @@
         <v>12</v>
       </c>
       <c r="C3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3" t="n">
         <v>50</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>54</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>36</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>48</v>
       </c>
     </row>
@@ -522,27 +535,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1m, 46s</t>
+          <t>54s</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>27m, 9s</t>
+          <t>32m, 19s</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>19m, 35s</t>
+          <t>15m, 45s</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>57m, 35s</t>
+          <t>13m, 12s</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>4h, 44m</t>
+          <t>47m, 36s</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1h, 26m</t>
         </is>
       </c>
     </row>
@@ -554,27 +572,32 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2s</t>
+          <t>1s</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1h, 46m</t>
+          <t>10m, 41s</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1h, 13m</t>
+          <t>1h, 1m</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2h, 22m</t>
+          <t>49m, 3s</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>18h, 46m</t>
+          <t>2h, 15m</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>5h, 41m</t>
         </is>
       </c>
     </row>
@@ -586,27 +609,32 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>6m, 14s</t>
+          <t>3m, 2s</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>24s</t>
+          <t>4s</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1m, 54s</t>
+          <t>15s</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1h, 20m</t>
+          <t>1m, 52s</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>21s</t>
+          <t>50m, 7s</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>6s</t>
         </is>
       </c>
     </row>

</xml_diff>